<commit_message>
File translade from Portuguese-Brazilian to English
</commit_message>
<xml_diff>
--- a/db-ciber-tri.xlsx
+++ b/db-ciber-tri.xlsx
@@ -1,17 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26122"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26207"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gills/Downloads/git-gills/2015-ciber-tri/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Total" sheetId="1" r:id="rId1"/>
-    <sheet name="Ciber" sheetId="3" r:id="rId2"/>
-    <sheet name="Ciber_TRI" sheetId="5" r:id="rId3"/>
+    <sheet name="Cyber" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -31,12 +35,11 @@
       <text>
         <r>
           <rPr>
-            <b/>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>não foram consideradas citações APENAS nas Referências</t>
+          <t>We do not count the citations contained only in references</t>
         </r>
       </text>
     </comment>
@@ -44,24 +47,11 @@
       <text>
         <r>
           <rPr>
-            <b/>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>valores rredondados</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E3" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>O CONCEITO DE REVOLUÇÃO NOS ASSUNTOS MILITARES (JOSÉ AUGUSTO ABREU DE MOURA)</t>
+          <t>rounding</t>
         </r>
       </text>
     </comment>
@@ -85,19 +75,7 @@
             <color indexed="81"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>os cinco, quatro referem-se ao setor cibernético da END</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F5" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>os cinco, quatro referem-se ao setor cibernético da END</t>
+          <t>Of the five papers, four refer to the cyber sector contained in the newly released Brazil's National Defense Strategy (END).</t>
         </r>
       </text>
     </comment>
@@ -109,7 +87,7 @@
             <color indexed="81"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t xml:space="preserve">http://seer.ufrgs.br/index.php/rbed/issue/view/2380/showToc
+          <t xml:space="preserve">Also available at: http://seer.ufrgs.br/index.php/rbed/issue/view/2380/showToc
 </t>
         </r>
       </text>
@@ -121,193 +99,10 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Gills</author>
     <author>Gills xx</author>
   </authors>
   <commentList>
-    <comment ref="C36" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">http://seer.ufrgs.br/index.php/rbed/issue/view/2380/showToc
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C37" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">http://seer.ufrgs.br/index.php/rbed/issue/view/2380/showToc
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C38" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">http://seer.ufrgs.br/index.php/rbed/issue/view/2380/showToc
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C39" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">http://seer.ufrgs.br/index.php/rbed/issue/view/2380/showToc
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C40" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">http://seer.ufrgs.br/index.php/rbed/issue/view/2380/showToc
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C41" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">http://seer.ufrgs.br/index.php/rbed/issue/view/2380/showToc
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C42" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">http://seer.ufrgs.br/index.php/rbed/issue/view/2380/showToc
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C43" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">http://seer.ufrgs.br/index.php/rbed/issue/view/2380/showToc
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C44" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">http://seer.ufrgs.br/index.php/rbed/issue/view/2380/showToc
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C45" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">http://seer.ufrgs.br/index.php/rbed/issue/view/2380/showToc
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C46" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">http://seer.ufrgs.br/index.php/rbed/issue/view/2380/showToc
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C47" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">http://seer.ufrgs.br/index.php/rbed/issue/view/2380/showToc
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C48" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">http://seer.ufrgs.br/index.php/rbed/issue/view/2380/showToc
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C49" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">http://seer.ufrgs.br/index.php/rbed/issue/view/2380/showToc
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G49" authorId="1">
+    <comment ref="H49" authorId="0">
       <text>
         <r>
           <rPr>
@@ -316,11 +111,11 @@
             <color indexed="81"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>O "Liberalismo" entrou por que utilizaram conceito do Joseph Nye.</t>
+          <t>"Liberalism" because the paper uses a Nye's concept</t>
         </r>
       </text>
     </comment>
-    <comment ref="C50" authorId="0">
+    <comment ref="D55" authorId="0">
       <text>
         <r>
           <rPr>
@@ -328,122 +123,7 @@
             <color indexed="81"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t xml:space="preserve">http://seer.ufrgs.br/index.php/rbed/issue/view/2380/showToc
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C51" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">http://seer.ufrgs.br/index.php/rbed/issue/view/2380/showToc
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C52" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">http://seer.ufrgs.br/index.php/rbed/issue/view/2380/showToc
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C53" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">http://seer.ufrgs.br/index.php/rbed/issue/view/2380/showToc
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D55" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>Apesar de manter o mesmo título de trabalho publicado nos anais de 2012, este é uma variação daquele.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Gills</author>
-    <author>Gills xx</author>
-  </authors>
-  <commentList>
-    <comment ref="C5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">http://seer.ufrgs.br/index.php/rbed/issue/view/2380/showToc
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C6" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">http://seer.ufrgs.br/index.php/rbed/issue/view/2380/showToc
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C7" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">http://seer.ufrgs.br/index.php/rbed/issue/view/2380/showToc
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G7" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>O "Liberalismo" entrou por que utilizaram conceito do Joseph Nye.</t>
+          <t>Although the paper to keep the same working title published in the proceedings of 2012, this is a variation of that.</t>
         </r>
       </text>
     </comment>
@@ -452,45 +132,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="130">
   <si>
     <t>ID</t>
   </si>
   <si>
-    <t>ANO</t>
-  </si>
-  <si>
     <t>PUB_TOTAL</t>
   </si>
   <si>
-    <t>PUB_CIBER</t>
-  </si>
-  <si>
-    <t>Não</t>
-  </si>
-  <si>
-    <t>Escola de Copenhague</t>
-  </si>
-  <si>
-    <t>CIBER_IMPORTÂNCIA</t>
-  </si>
-  <si>
-    <t>CIBER_TEORIA</t>
-  </si>
-  <si>
     <t>Limites e perspectivas da securitização: estudos de caso no contexto sulamericano contemporâneo</t>
   </si>
   <si>
-    <t>PUBLICAÇÃO_TÍTULO</t>
-  </si>
-  <si>
     <t>O conceito de Revolução nos Assuntos Militares</t>
   </si>
   <si>
     <t>José Augusto Abreu de Moura</t>
-  </si>
-  <si>
-    <t>AUTORIA</t>
   </si>
   <si>
     <t>O Parlamento e a Política de Defesa Nacional</t>
@@ -707,9 +363,6 @@
     <t>Walfredo Bento Ferreira Neto</t>
   </si>
   <si>
-    <t>Realismo; Escola Inglesa</t>
-  </si>
-  <si>
     <t>A geopolítica da América do Sul: o papel determinante da Defesa na integração do setor elétrico</t>
   </si>
   <si>
@@ -773,9 +426,6 @@
     <t>Luiz Felipe Rebello</t>
   </si>
   <si>
-    <t>Escola de Copenhague, Liberalismo</t>
-  </si>
-  <si>
     <t>Novas ameaças no século XXI: o terrorismo transnacional</t>
   </si>
   <si>
@@ -791,9 +441,6 @@
     <t>Genessi Sá Junior; Rui Martins da Motta</t>
   </si>
   <si>
-    <t>Liberalismo; Escola de Copenhague</t>
-  </si>
-  <si>
     <t>O terrorismo na América do Sul e a segurança regional comparada</t>
   </si>
   <si>
@@ -851,7 +498,43 @@
     <t>TOTAL</t>
   </si>
   <si>
-    <t>Sim</t>
+    <t>YEAR</t>
+  </si>
+  <si>
+    <t>PUB_CYBER</t>
+  </si>
+  <si>
+    <t>AUTORSHIP</t>
+  </si>
+  <si>
+    <t>TITLE</t>
+  </si>
+  <si>
+    <t>CYBER_SIGNIFICANCE</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>CYBER_AND_THEORY</t>
+  </si>
+  <si>
+    <t>THEORY</t>
+  </si>
+  <si>
+    <t>Copenhagen School</t>
+  </si>
+  <si>
+    <t>Realism; English School</t>
+  </si>
+  <si>
+    <t>Liberalism; Copenhagen School</t>
+  </si>
+  <si>
+    <t>Copenhagen School; Liberalism</t>
   </si>
 </sst>
 </file>
@@ -1344,7 +1027,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1462,183 +1145,177 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="3" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="3" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="88">
-    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="36" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="40" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="64" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="66" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="68" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="74" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="82" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="87" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -1905,7 +1582,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1916,11 +1593,11 @@
   <sheetPr codeName="Plan1" enableFormatConditionsCalculation="0"/>
   <dimension ref="B1:F10"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="2" max="2" width="10.83203125" style="2"/>
@@ -1930,25 +1607,25 @@
     <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="16" thickBot="1"/>
-    <row r="2" spans="2:6" s="3" customFormat="1" ht="16" thickBot="1">
+    <row r="1" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:6" s="3" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="34" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="D2" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="35" t="s">
-        <v>2</v>
-      </c>
       <c r="E2" s="36" t="s">
-        <v>3</v>
+        <v>118</v>
       </c>
       <c r="F2" s="37" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" s="24">
         <v>1</v>
       </c>
@@ -1959,34 +1636,34 @@
         <f>9+9+6+6+6+5+3+4+5+6+5+10+4+5+4+7</f>
         <v>94</v>
       </c>
-      <c r="E3" s="48">
+      <c r="E3" s="46">
         <v>1</v>
       </c>
-      <c r="F3" s="44">
+      <c r="F3" s="42">
         <f>E3/D3</f>
         <v>1.0638297872340425E-2</v>
       </c>
     </row>
-    <row r="4" spans="2:6">
-      <c r="B4" s="50">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B4" s="48">
         <v>2</v>
       </c>
-      <c r="C4" s="51">
+      <c r="C4" s="49">
         <v>2008</v>
       </c>
-      <c r="D4" s="51">
+      <c r="D4" s="49">
         <f>12+6+5+4+5+6+11+16</f>
         <v>65</v>
       </c>
-      <c r="E4" s="52">
+      <c r="E4" s="50">
         <v>2</v>
       </c>
-      <c r="F4" s="53">
+      <c r="F4" s="51">
         <f>E4/D4</f>
         <v>3.0769230769230771E-2</v>
       </c>
     </row>
-    <row r="5" spans="2:6">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5" s="5">
         <v>3</v>
       </c>
@@ -1996,34 +1673,34 @@
       <c r="D5" s="6">
         <v>45</v>
       </c>
-      <c r="E5" s="49">
+      <c r="E5" s="47">
         <v>5</v>
       </c>
-      <c r="F5" s="45">
+      <c r="F5" s="43">
         <f t="shared" ref="F5:F9" si="0">E5/D5</f>
         <v>0.1111111111111111</v>
       </c>
     </row>
-    <row r="6" spans="2:6">
-      <c r="B6" s="50">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B6" s="48">
         <v>4</v>
       </c>
-      <c r="C6" s="51">
+      <c r="C6" s="49">
         <v>2010</v>
       </c>
-      <c r="D6" s="51">
+      <c r="D6" s="49">
         <f>1+5+8+7+9+11+11+17</f>
         <v>69</v>
       </c>
-      <c r="E6" s="52">
+      <c r="E6" s="50">
         <v>10</v>
       </c>
-      <c r="F6" s="53">
+      <c r="F6" s="51">
         <f t="shared" si="0"/>
         <v>0.14492753623188406</v>
       </c>
     </row>
-    <row r="7" spans="2:6">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B7" s="5">
         <v>5</v>
       </c>
@@ -2034,34 +1711,34 @@
         <f>9+12+13+10+7+5+5+18+6+13+10+12+10+14+15</f>
         <v>159</v>
       </c>
-      <c r="E7" s="49">
+      <c r="E7" s="47">
         <v>15</v>
       </c>
-      <c r="F7" s="45">
+      <c r="F7" s="43">
         <f t="shared" si="0"/>
         <v>9.4339622641509441E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:6">
-      <c r="B8" s="50">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B8" s="48">
         <v>6</v>
       </c>
-      <c r="C8" s="51">
+      <c r="C8" s="49">
         <v>2012</v>
       </c>
-      <c r="D8" s="51">
+      <c r="D8" s="49">
         <f>11+7+3+15+7+4+9+3+7+5+6+4+7+5+6+5+13+13+12+8+5+4</f>
         <v>159</v>
       </c>
-      <c r="E8" s="52">
+      <c r="E8" s="50">
         <v>18</v>
       </c>
-      <c r="F8" s="53">
+      <c r="F8" s="51">
         <f t="shared" si="0"/>
         <v>0.11320754716981132</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="16" thickBot="1">
+    <row r="9" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="39">
         <v>7</v>
       </c>
@@ -2074,16 +1751,16 @@
       <c r="E9" s="40">
         <v>9</v>
       </c>
-      <c r="F9" s="46">
+      <c r="F9" s="44">
         <f t="shared" si="0"/>
         <v>0.12162162162162163</v>
       </c>
     </row>
-    <row r="10" spans="2:6" s="38" customFormat="1" ht="16" thickBot="1">
-      <c r="B10" s="41" t="s">
-        <v>127</v>
-      </c>
-      <c r="C10" s="42"/>
+    <row r="10" spans="2:6" s="38" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="66" t="s">
+        <v>116</v>
+      </c>
+      <c r="C10" s="67"/>
       <c r="D10" s="4">
         <f>SUM(D3:D9)</f>
         <v>665</v>
@@ -2092,7 +1769,7 @@
         <f>SUM(E3:E9)</f>
         <v>60</v>
       </c>
-      <c r="F10" s="47">
+      <c r="F10" s="45">
         <f>E10/D10</f>
         <v>9.0225563909774431E-2</v>
       </c>
@@ -2103,24 +1780,19 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Plan2" enableFormatConditionsCalculation="0"/>
-  <dimension ref="B1:G62"/>
+  <dimension ref="B1:H62"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="G63" sqref="G63"/>
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.33203125" style="15" customWidth="1"/>
     <col min="2" max="2" width="5.1640625" style="14" customWidth="1"/>
@@ -2128,32 +1800,35 @@
     <col min="4" max="4" width="49.6640625" style="7" customWidth="1"/>
     <col min="5" max="5" width="30" style="7" customWidth="1"/>
     <col min="6" max="6" width="19.33203125" style="14" customWidth="1"/>
-    <col min="7" max="7" width="19.83203125" style="14" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="15"/>
+    <col min="7" max="8" width="19.83203125" style="14" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="16" thickBot="1"/>
-    <row r="2" spans="2:7" s="16" customFormat="1" ht="16" thickBot="1">
+    <row r="1" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:8" s="16" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="26" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>1</v>
+        <v>117</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>9</v>
+        <v>120</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>12</v>
+        <v>119</v>
       </c>
       <c r="F2" s="28" t="s">
-        <v>6</v>
+        <v>121</v>
       </c>
       <c r="G2" s="29" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7">
+        <v>124</v>
+      </c>
+      <c r="H2" s="29" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B3" s="30">
         <v>1</v>
       </c>
@@ -2161,39 +1836,41 @@
         <v>2007</v>
       </c>
       <c r="D3" s="32" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E3" s="32" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="F3" s="31">
         <v>0</v>
       </c>
       <c r="G3" s="33" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" ht="30">
-      <c r="B4" s="54">
+        <v>122</v>
+      </c>
+      <c r="H3" s="33"/>
+    </row>
+    <row r="4" spans="2:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="B4" s="52">
         <v>2</v>
       </c>
-      <c r="C4" s="55">
+      <c r="C4" s="53">
         <v>2008</v>
       </c>
-      <c r="D4" s="56" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="56" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="55">
-        <v>0</v>
-      </c>
-      <c r="G4" s="57" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" ht="30">
+      <c r="D4" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="54" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="53">
+        <v>0</v>
+      </c>
+      <c r="G4" s="55" t="s">
+        <v>122</v>
+      </c>
+      <c r="H4" s="55"/>
+    </row>
+    <row r="5" spans="2:8" ht="32" x14ac:dyDescent="0.2">
       <c r="B5" s="17">
         <v>3</v>
       </c>
@@ -2201,39 +1878,41 @@
         <v>2008</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="F5" s="18">
         <v>0</v>
       </c>
       <c r="G5" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="H5" s="19"/>
+    </row>
+    <row r="6" spans="2:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="B6" s="52">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="2:7" ht="30">
-      <c r="B6" s="54">
-        <v>4</v>
-      </c>
-      <c r="C6" s="55">
+      <c r="C6" s="53">
         <v>2009</v>
       </c>
-      <c r="D6" s="56" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="56" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="55">
-        <v>0</v>
-      </c>
-      <c r="G6" s="57" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" ht="45">
+      <c r="D6" s="54" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="54" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="53">
+        <v>0</v>
+      </c>
+      <c r="G6" s="55" t="s">
+        <v>122</v>
+      </c>
+      <c r="H6" s="55"/>
+    </row>
+    <row r="7" spans="2:8" ht="48" x14ac:dyDescent="0.2">
       <c r="B7" s="17">
         <v>5</v>
       </c>
@@ -2241,39 +1920,41 @@
         <v>2009</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="F7" s="18">
         <v>0</v>
       </c>
       <c r="G7" s="19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" ht="30">
-      <c r="B8" s="54">
+        <v>122</v>
+      </c>
+      <c r="H7" s="19"/>
+    </row>
+    <row r="8" spans="2:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="B8" s="52">
         <v>6</v>
       </c>
-      <c r="C8" s="55">
+      <c r="C8" s="53">
         <v>2009</v>
       </c>
-      <c r="D8" s="56" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="56" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="55">
-        <v>0</v>
-      </c>
-      <c r="G8" s="57" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" ht="30">
+      <c r="D8" s="54" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="54" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="53">
+        <v>0</v>
+      </c>
+      <c r="G8" s="55" t="s">
+        <v>122</v>
+      </c>
+      <c r="H8" s="55"/>
+    </row>
+    <row r="9" spans="2:8" ht="32" x14ac:dyDescent="0.2">
       <c r="B9" s="17">
         <v>7</v>
       </c>
@@ -2281,39 +1962,41 @@
         <v>2009</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="F9" s="18">
         <v>0</v>
       </c>
       <c r="G9" s="19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7">
-      <c r="B10" s="54">
+        <v>122</v>
+      </c>
+      <c r="H9" s="19"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B10" s="52">
         <v>8</v>
       </c>
-      <c r="C10" s="55">
+      <c r="C10" s="53">
         <v>2009</v>
       </c>
-      <c r="D10" s="56" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="56" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10" s="55">
-        <v>0</v>
-      </c>
-      <c r="G10" s="57" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" ht="30">
+      <c r="D10" s="54" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="54" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="53">
+        <v>0</v>
+      </c>
+      <c r="G10" s="55" t="s">
+        <v>122</v>
+      </c>
+      <c r="H10" s="55"/>
+    </row>
+    <row r="11" spans="2:8" ht="32" x14ac:dyDescent="0.2">
       <c r="B11" s="17">
         <v>9</v>
       </c>
@@ -2321,39 +2004,41 @@
         <v>2010</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="F11" s="18">
         <v>0</v>
       </c>
       <c r="G11" s="19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" ht="30">
-      <c r="B12" s="54">
+        <v>122</v>
+      </c>
+      <c r="H11" s="19"/>
+    </row>
+    <row r="12" spans="2:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="B12" s="52">
         <v>10</v>
       </c>
-      <c r="C12" s="55">
+      <c r="C12" s="53">
         <v>2010</v>
       </c>
-      <c r="D12" s="56" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="56" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12" s="55">
-        <v>0</v>
-      </c>
-      <c r="G12" s="57" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" ht="30">
+      <c r="D12" s="54" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="54" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="53">
+        <v>0</v>
+      </c>
+      <c r="G12" s="55" t="s">
+        <v>122</v>
+      </c>
+      <c r="H12" s="55"/>
+    </row>
+    <row r="13" spans="2:8" ht="32" x14ac:dyDescent="0.2">
       <c r="B13" s="17">
         <v>11</v>
       </c>
@@ -2361,39 +2046,41 @@
         <v>2010</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="F13" s="18">
         <v>0</v>
       </c>
       <c r="G13" s="19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" ht="30">
-      <c r="B14" s="54">
+        <v>122</v>
+      </c>
+      <c r="H13" s="19"/>
+    </row>
+    <row r="14" spans="2:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="B14" s="52">
         <v>12</v>
       </c>
-      <c r="C14" s="55">
+      <c r="C14" s="53">
         <v>2010</v>
       </c>
-      <c r="D14" s="58" t="s">
-        <v>35</v>
-      </c>
-      <c r="E14" s="56" t="s">
-        <v>36</v>
-      </c>
-      <c r="F14" s="55">
-        <v>0</v>
-      </c>
-      <c r="G14" s="57" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" ht="30">
+      <c r="D14" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="53">
+        <v>0</v>
+      </c>
+      <c r="G14" s="55" t="s">
+        <v>122</v>
+      </c>
+      <c r="H14" s="55"/>
+    </row>
+    <row r="15" spans="2:8" ht="32" x14ac:dyDescent="0.2">
       <c r="B15" s="17">
         <v>13</v>
       </c>
@@ -2401,39 +2088,41 @@
         <v>2010</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="F15" s="18">
         <v>0</v>
       </c>
       <c r="G15" s="19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" ht="30">
-      <c r="B16" s="54">
+        <v>122</v>
+      </c>
+      <c r="H15" s="19"/>
+    </row>
+    <row r="16" spans="2:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="B16" s="52">
         <v>14</v>
       </c>
-      <c r="C16" s="55">
+      <c r="C16" s="53">
         <v>2010</v>
       </c>
-      <c r="D16" s="56" t="s">
-        <v>39</v>
-      </c>
-      <c r="E16" s="56" t="s">
-        <v>40</v>
-      </c>
-      <c r="F16" s="55">
-        <v>0</v>
-      </c>
-      <c r="G16" s="57" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" ht="30">
+      <c r="D16" s="54" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="54" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="53">
+        <v>0</v>
+      </c>
+      <c r="G16" s="55" t="s">
+        <v>122</v>
+      </c>
+      <c r="H16" s="55"/>
+    </row>
+    <row r="17" spans="2:8" ht="32" x14ac:dyDescent="0.2">
       <c r="B17" s="17">
         <v>15</v>
       </c>
@@ -2441,39 +2130,41 @@
         <v>2010</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F17" s="18">
         <v>0</v>
       </c>
       <c r="G17" s="19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" ht="45">
-      <c r="B18" s="54">
+        <v>122</v>
+      </c>
+      <c r="H17" s="19"/>
+    </row>
+    <row r="18" spans="2:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="B18" s="52">
         <v>16</v>
       </c>
-      <c r="C18" s="55">
+      <c r="C18" s="53">
         <v>2010</v>
       </c>
-      <c r="D18" s="56" t="s">
-        <v>42</v>
-      </c>
-      <c r="E18" s="56" t="s">
-        <v>43</v>
-      </c>
-      <c r="F18" s="55">
-        <v>0</v>
-      </c>
-      <c r="G18" s="57" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" ht="30">
+      <c r="D18" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" s="53">
+        <v>0</v>
+      </c>
+      <c r="G18" s="55" t="s">
+        <v>122</v>
+      </c>
+      <c r="H18" s="55"/>
+    </row>
+    <row r="19" spans="2:8" ht="32" x14ac:dyDescent="0.2">
       <c r="B19" s="17">
         <v>17</v>
       </c>
@@ -2481,39 +2172,41 @@
         <v>2010</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="F19" s="18">
         <v>0</v>
       </c>
       <c r="G19" s="19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" ht="30">
-      <c r="B20" s="54">
+        <v>122</v>
+      </c>
+      <c r="H19" s="19"/>
+    </row>
+    <row r="20" spans="2:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="B20" s="52">
         <v>18</v>
       </c>
-      <c r="C20" s="55">
+      <c r="C20" s="53">
         <v>2010</v>
       </c>
-      <c r="D20" s="56" t="s">
-        <v>46</v>
-      </c>
-      <c r="E20" s="56" t="s">
-        <v>47</v>
-      </c>
-      <c r="F20" s="55">
-        <v>0</v>
-      </c>
-      <c r="G20" s="57" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" ht="30">
+      <c r="D20" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" s="54" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" s="53">
+        <v>0</v>
+      </c>
+      <c r="G20" s="55" t="s">
+        <v>122</v>
+      </c>
+      <c r="H20" s="55"/>
+    </row>
+    <row r="21" spans="2:8" ht="32" x14ac:dyDescent="0.2">
       <c r="B21" s="17">
         <v>19</v>
       </c>
@@ -2521,39 +2214,41 @@
         <v>2011</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="F21" s="18">
         <v>0</v>
       </c>
       <c r="G21" s="19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7">
-      <c r="B22" s="54">
+        <v>122</v>
+      </c>
+      <c r="H21" s="19"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B22" s="52">
         <v>20</v>
       </c>
-      <c r="C22" s="55">
+      <c r="C22" s="53">
         <v>2011</v>
       </c>
-      <c r="D22" s="59" t="s">
-        <v>51</v>
-      </c>
-      <c r="E22" s="60" t="s">
-        <v>52</v>
-      </c>
-      <c r="F22" s="55">
+      <c r="D22" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="58" t="s">
+        <v>44</v>
+      </c>
+      <c r="F22" s="53">
         <v>2</v>
       </c>
-      <c r="G22" s="57" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" ht="30">
+      <c r="G22" s="55" t="s">
+        <v>122</v>
+      </c>
+      <c r="H22" s="55"/>
+    </row>
+    <row r="23" spans="2:8" ht="32" x14ac:dyDescent="0.2">
       <c r="B23" s="17">
         <v>21</v>
       </c>
@@ -2561,39 +2256,43 @@
         <v>2011</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="F23" s="18">
         <v>2</v>
       </c>
       <c r="G23" s="19" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7">
-      <c r="B24" s="54">
+        <v>123</v>
+      </c>
+      <c r="H23" s="19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B24" s="52">
         <v>22</v>
       </c>
-      <c r="C24" s="55">
+      <c r="C24" s="53">
         <v>2011</v>
       </c>
-      <c r="D24" s="60" t="s">
-        <v>55</v>
-      </c>
-      <c r="E24" s="58" t="s">
-        <v>56</v>
-      </c>
-      <c r="F24" s="55">
-        <v>0</v>
-      </c>
-      <c r="G24" s="57" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" ht="30">
+      <c r="D24" s="58" t="s">
+        <v>47</v>
+      </c>
+      <c r="E24" s="56" t="s">
+        <v>48</v>
+      </c>
+      <c r="F24" s="53">
+        <v>0</v>
+      </c>
+      <c r="G24" s="55" t="s">
+        <v>122</v>
+      </c>
+      <c r="H24" s="55"/>
+    </row>
+    <row r="25" spans="2:8" ht="32" x14ac:dyDescent="0.2">
       <c r="B25" s="17">
         <v>23</v>
       </c>
@@ -2601,39 +2300,41 @@
         <v>2011</v>
       </c>
       <c r="D25" s="21" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="F25" s="18">
         <v>0</v>
       </c>
       <c r="G25" s="19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" ht="42">
-      <c r="B26" s="54">
+        <v>122</v>
+      </c>
+      <c r="H25" s="19"/>
+    </row>
+    <row r="26" spans="2:8" ht="45" x14ac:dyDescent="0.2">
+      <c r="B26" s="52">
         <v>24</v>
       </c>
-      <c r="C26" s="55">
+      <c r="C26" s="53">
         <v>2011</v>
       </c>
-      <c r="D26" s="61" t="s">
-        <v>59</v>
-      </c>
-      <c r="E26" s="61" t="s">
-        <v>60</v>
-      </c>
-      <c r="F26" s="55">
-        <v>0</v>
-      </c>
-      <c r="G26" s="57" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" ht="30">
+      <c r="D26" s="59" t="s">
+        <v>51</v>
+      </c>
+      <c r="E26" s="59" t="s">
+        <v>52</v>
+      </c>
+      <c r="F26" s="53">
+        <v>0</v>
+      </c>
+      <c r="G26" s="55" t="s">
+        <v>122</v>
+      </c>
+      <c r="H26" s="55"/>
+    </row>
+    <row r="27" spans="2:8" ht="32" x14ac:dyDescent="0.2">
       <c r="B27" s="17">
         <v>25</v>
       </c>
@@ -2641,39 +2342,41 @@
         <v>2011</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="F27" s="18">
         <v>0</v>
       </c>
       <c r="G27" s="19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" ht="45">
-      <c r="B28" s="54">
+        <v>122</v>
+      </c>
+      <c r="H27" s="19"/>
+    </row>
+    <row r="28" spans="2:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="B28" s="52">
         <v>26</v>
       </c>
-      <c r="C28" s="55">
+      <c r="C28" s="53">
         <v>2011</v>
       </c>
-      <c r="D28" s="56" t="s">
-        <v>63</v>
-      </c>
-      <c r="E28" s="62" t="s">
-        <v>64</v>
-      </c>
-      <c r="F28" s="55">
-        <v>0</v>
-      </c>
-      <c r="G28" s="57" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" ht="45">
+      <c r="D28" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="E28" s="60" t="s">
+        <v>56</v>
+      </c>
+      <c r="F28" s="53">
+        <v>0</v>
+      </c>
+      <c r="G28" s="55" t="s">
+        <v>123</v>
+      </c>
+      <c r="H28" s="55"/>
+    </row>
+    <row r="29" spans="2:8" ht="48" x14ac:dyDescent="0.2">
       <c r="B29" s="17">
         <v>27</v>
       </c>
@@ -2681,39 +2384,43 @@
         <v>2011</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="E29" s="23" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="F29" s="18">
         <v>2</v>
       </c>
       <c r="G29" s="19" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7">
-      <c r="B30" s="54">
+        <v>123</v>
+      </c>
+      <c r="H29" s="19" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B30" s="52">
         <v>28</v>
       </c>
-      <c r="C30" s="55">
+      <c r="C30" s="53">
         <v>2011</v>
       </c>
-      <c r="D30" s="60" t="s">
-        <v>66</v>
-      </c>
-      <c r="E30" s="60" t="s">
-        <v>67</v>
-      </c>
-      <c r="F30" s="55">
-        <v>0</v>
-      </c>
-      <c r="G30" s="57" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" ht="30">
+      <c r="D30" s="58" t="s">
+        <v>58</v>
+      </c>
+      <c r="E30" s="58" t="s">
+        <v>59</v>
+      </c>
+      <c r="F30" s="53">
+        <v>0</v>
+      </c>
+      <c r="G30" s="55" t="s">
+        <v>122</v>
+      </c>
+      <c r="H30" s="55"/>
+    </row>
+    <row r="31" spans="2:8" ht="32" x14ac:dyDescent="0.2">
       <c r="B31" s="17">
         <v>29</v>
       </c>
@@ -2721,39 +2428,41 @@
         <v>2011</v>
       </c>
       <c r="D31" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="E31" s="43" t="s">
-        <v>69</v>
+        <v>60</v>
+      </c>
+      <c r="E31" s="41" t="s">
+        <v>61</v>
       </c>
       <c r="F31" s="18">
         <v>0</v>
       </c>
       <c r="G31" s="19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" ht="45">
-      <c r="B32" s="54">
+        <v>122</v>
+      </c>
+      <c r="H31" s="19"/>
+    </row>
+    <row r="32" spans="2:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="B32" s="52">
         <v>30</v>
       </c>
-      <c r="C32" s="55">
+      <c r="C32" s="53">
         <v>2011</v>
       </c>
-      <c r="D32" s="63" t="s">
-        <v>70</v>
-      </c>
-      <c r="E32" s="60" t="s">
-        <v>71</v>
-      </c>
-      <c r="F32" s="55">
-        <v>0</v>
-      </c>
-      <c r="G32" s="57" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7">
+      <c r="D32" s="61" t="s">
+        <v>62</v>
+      </c>
+      <c r="E32" s="58" t="s">
+        <v>63</v>
+      </c>
+      <c r="F32" s="53">
+        <v>0</v>
+      </c>
+      <c r="G32" s="55" t="s">
+        <v>122</v>
+      </c>
+      <c r="H32" s="55"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B33" s="17">
         <v>31</v>
       </c>
@@ -2761,39 +2470,41 @@
         <v>2011</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E33" s="13" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="F33" s="18">
         <v>0</v>
       </c>
       <c r="G33" s="19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" ht="33" customHeight="1">
-      <c r="B34" s="54">
+        <v>122</v>
+      </c>
+      <c r="H33" s="19"/>
+    </row>
+    <row r="34" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="52">
         <v>32</v>
       </c>
-      <c r="C34" s="55">
+      <c r="C34" s="53">
         <v>2011</v>
       </c>
-      <c r="D34" s="56" t="s">
-        <v>74</v>
-      </c>
-      <c r="E34" s="56" t="s">
-        <v>75</v>
-      </c>
-      <c r="F34" s="55">
-        <v>0</v>
-      </c>
-      <c r="G34" s="57" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7">
+      <c r="D34" s="54" t="s">
+        <v>66</v>
+      </c>
+      <c r="E34" s="54" t="s">
+        <v>67</v>
+      </c>
+      <c r="F34" s="53">
+        <v>0</v>
+      </c>
+      <c r="G34" s="55" t="s">
+        <v>122</v>
+      </c>
+      <c r="H34" s="55"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B35" s="17">
         <v>33</v>
       </c>
@@ -2801,39 +2512,43 @@
         <v>2011</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="E35" s="23" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="F35" s="18">
         <v>0</v>
       </c>
       <c r="G35" s="19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="2:7" ht="30">
-      <c r="B36" s="54">
+        <v>122</v>
+      </c>
+      <c r="H35" s="19"/>
+    </row>
+    <row r="36" spans="2:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="B36" s="52">
         <v>34</v>
       </c>
-      <c r="C36" s="55">
+      <c r="C36" s="53">
         <v>2012</v>
       </c>
-      <c r="D36" s="62" t="s">
-        <v>78</v>
-      </c>
-      <c r="E36" s="60" t="s">
-        <v>79</v>
-      </c>
-      <c r="F36" s="55">
+      <c r="D36" s="60" t="s">
+        <v>70</v>
+      </c>
+      <c r="E36" s="58" t="s">
+        <v>71</v>
+      </c>
+      <c r="F36" s="53">
         <v>2</v>
       </c>
-      <c r="G36" s="57" t="s">
+      <c r="G36" s="55" t="s">
+        <v>123</v>
+      </c>
+      <c r="H36" s="55" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="37" spans="2:7" ht="30">
+    <row r="37" spans="2:8" ht="32" x14ac:dyDescent="0.2">
       <c r="B37" s="17">
         <v>35</v>
       </c>
@@ -2841,39 +2556,41 @@
         <v>2012</v>
       </c>
       <c r="D37" s="20" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="E37" s="23" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F37" s="18">
         <v>1</v>
       </c>
       <c r="G37" s="19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="2:7" ht="45">
-      <c r="B38" s="54">
+        <v>122</v>
+      </c>
+      <c r="H37" s="19"/>
+    </row>
+    <row r="38" spans="2:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="B38" s="52">
         <v>36</v>
       </c>
-      <c r="C38" s="55">
+      <c r="C38" s="53">
         <v>2012</v>
       </c>
-      <c r="D38" s="56" t="s">
-        <v>13</v>
-      </c>
-      <c r="E38" s="56" t="s">
-        <v>14</v>
-      </c>
-      <c r="F38" s="55">
-        <v>0</v>
-      </c>
-      <c r="G38" s="57" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39" spans="2:7" ht="30">
+      <c r="D38" s="54" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38" s="54" t="s">
+        <v>6</v>
+      </c>
+      <c r="F38" s="53">
+        <v>0</v>
+      </c>
+      <c r="G38" s="55" t="s">
+        <v>122</v>
+      </c>
+      <c r="H38" s="55"/>
+    </row>
+    <row r="39" spans="2:8" ht="32" x14ac:dyDescent="0.2">
       <c r="B39" s="17">
         <v>37</v>
       </c>
@@ -2881,39 +2598,41 @@
         <v>2012</v>
       </c>
       <c r="D39" s="20" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="F39" s="18">
         <v>0</v>
       </c>
       <c r="G39" s="19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="2:7" ht="30">
-      <c r="B40" s="54">
+        <v>122</v>
+      </c>
+      <c r="H39" s="19"/>
+    </row>
+    <row r="40" spans="2:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="B40" s="52">
         <v>38</v>
       </c>
-      <c r="C40" s="55">
+      <c r="C40" s="53">
         <v>2012</v>
       </c>
-      <c r="D40" s="58" t="s">
-        <v>86</v>
-      </c>
-      <c r="E40" s="56" t="s">
-        <v>28</v>
-      </c>
-      <c r="F40" s="55">
-        <v>0</v>
-      </c>
-      <c r="G40" s="57" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="2:7" ht="45">
+      <c r="D40" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="E40" s="54" t="s">
+        <v>20</v>
+      </c>
+      <c r="F40" s="53">
+        <v>0</v>
+      </c>
+      <c r="G40" s="55" t="s">
+        <v>122</v>
+      </c>
+      <c r="H40" s="55"/>
+    </row>
+    <row r="41" spans="2:8" ht="48" x14ac:dyDescent="0.2">
       <c r="B41" s="17">
         <v>39</v>
       </c>
@@ -2921,39 +2640,41 @@
         <v>2012</v>
       </c>
       <c r="D41" s="20" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="E41" s="23" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="F41" s="18">
         <v>0</v>
       </c>
       <c r="G41" s="19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="2:7" ht="30">
-      <c r="B42" s="54">
+        <v>122</v>
+      </c>
+      <c r="H41" s="19"/>
+    </row>
+    <row r="42" spans="2:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="B42" s="52">
         <v>40</v>
       </c>
-      <c r="C42" s="55">
+      <c r="C42" s="53">
         <v>2012</v>
       </c>
-      <c r="D42" s="58" t="s">
-        <v>88</v>
-      </c>
-      <c r="E42" s="60" t="s">
-        <v>89</v>
-      </c>
-      <c r="F42" s="55">
-        <v>0</v>
-      </c>
-      <c r="G42" s="57" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="2:7" ht="30">
+      <c r="D42" s="56" t="s">
+        <v>79</v>
+      </c>
+      <c r="E42" s="58" t="s">
+        <v>80</v>
+      </c>
+      <c r="F42" s="53">
+        <v>0</v>
+      </c>
+      <c r="G42" s="55" t="s">
+        <v>122</v>
+      </c>
+      <c r="H42" s="55"/>
+    </row>
+    <row r="43" spans="2:8" ht="32" x14ac:dyDescent="0.2">
       <c r="B43" s="17">
         <v>41</v>
       </c>
@@ -2961,39 +2682,41 @@
         <v>2012</v>
       </c>
       <c r="D43" s="20" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="E43" s="23" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="F43" s="18">
         <v>0</v>
       </c>
       <c r="G43" s="19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="2:7" ht="45">
-      <c r="B44" s="54">
+        <v>122</v>
+      </c>
+      <c r="H43" s="19"/>
+    </row>
+    <row r="44" spans="2:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="B44" s="52">
         <v>42</v>
       </c>
-      <c r="C44" s="55">
+      <c r="C44" s="53">
         <v>2012</v>
       </c>
-      <c r="D44" s="58" t="s">
-        <v>92</v>
-      </c>
-      <c r="E44" s="60" t="s">
-        <v>93</v>
-      </c>
-      <c r="F44" s="55">
-        <v>0</v>
-      </c>
-      <c r="G44" s="57" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="2:7" ht="30">
+      <c r="D44" s="56" t="s">
+        <v>83</v>
+      </c>
+      <c r="E44" s="58" t="s">
+        <v>84</v>
+      </c>
+      <c r="F44" s="53">
+        <v>0</v>
+      </c>
+      <c r="G44" s="55" t="s">
+        <v>122</v>
+      </c>
+      <c r="H44" s="55"/>
+    </row>
+    <row r="45" spans="2:8" ht="32" x14ac:dyDescent="0.2">
       <c r="B45" s="17">
         <v>43</v>
       </c>
@@ -3001,39 +2724,41 @@
         <v>2012</v>
       </c>
       <c r="D45" s="20" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="E45" s="23" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="F45" s="18">
         <v>1</v>
       </c>
       <c r="G45" s="19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="46" spans="2:7" ht="30">
-      <c r="B46" s="54">
+        <v>122</v>
+      </c>
+      <c r="H45" s="19"/>
+    </row>
+    <row r="46" spans="2:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="B46" s="52">
         <v>44</v>
       </c>
-      <c r="C46" s="55">
+      <c r="C46" s="53">
         <v>2012</v>
       </c>
-      <c r="D46" s="58" t="s">
-        <v>96</v>
-      </c>
-      <c r="E46" s="60" t="s">
-        <v>97</v>
-      </c>
-      <c r="F46" s="55">
+      <c r="D46" s="56" t="s">
+        <v>87</v>
+      </c>
+      <c r="E46" s="58" t="s">
+        <v>88</v>
+      </c>
+      <c r="F46" s="53">
         <v>2</v>
       </c>
-      <c r="G46" s="57" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="47" spans="2:7" ht="30">
+      <c r="G46" s="55" t="s">
+        <v>122</v>
+      </c>
+      <c r="H46" s="55"/>
+    </row>
+    <row r="47" spans="2:8" ht="32" x14ac:dyDescent="0.2">
       <c r="B47" s="17">
         <v>45</v>
       </c>
@@ -3041,39 +2766,43 @@
         <v>2012</v>
       </c>
       <c r="D47" s="20" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="E47" s="23" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="F47" s="18">
         <v>2</v>
       </c>
       <c r="G47" s="19" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="48" spans="2:7" ht="30">
-      <c r="B48" s="54">
+        <v>123</v>
+      </c>
+      <c r="H47" s="19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="B48" s="52">
         <v>46</v>
       </c>
-      <c r="C48" s="55">
+      <c r="C48" s="53">
         <v>2012</v>
       </c>
-      <c r="D48" s="58" t="s">
-        <v>100</v>
-      </c>
-      <c r="E48" s="60" t="s">
-        <v>101</v>
-      </c>
-      <c r="F48" s="55">
-        <v>0</v>
-      </c>
-      <c r="G48" s="57" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="49" spans="2:7" ht="45">
+      <c r="D48" s="56" t="s">
+        <v>91</v>
+      </c>
+      <c r="E48" s="58" t="s">
+        <v>92</v>
+      </c>
+      <c r="F48" s="53">
+        <v>0</v>
+      </c>
+      <c r="G48" s="55" t="s">
+        <v>122</v>
+      </c>
+      <c r="H48" s="55"/>
+    </row>
+    <row r="49" spans="2:8" ht="48" x14ac:dyDescent="0.2">
       <c r="B49" s="17">
         <v>47</v>
       </c>
@@ -3081,39 +2810,43 @@
         <v>2012</v>
       </c>
       <c r="D49" s="10" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E49" s="10" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="F49" s="18">
         <v>1</v>
       </c>
       <c r="G49" s="19" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="50" spans="2:7">
-      <c r="B50" s="54">
+        <v>123</v>
+      </c>
+      <c r="H49" s="19" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B50" s="52">
         <v>48</v>
       </c>
-      <c r="C50" s="55">
+      <c r="C50" s="53">
         <v>2012</v>
       </c>
-      <c r="D50" s="58" t="s">
-        <v>103</v>
-      </c>
-      <c r="E50" s="60" t="s">
-        <v>104</v>
-      </c>
-      <c r="F50" s="55">
-        <v>0</v>
-      </c>
-      <c r="G50" s="57" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="51" spans="2:7" ht="30">
+      <c r="D50" s="56" t="s">
+        <v>93</v>
+      </c>
+      <c r="E50" s="58" t="s">
+        <v>94</v>
+      </c>
+      <c r="F50" s="53">
+        <v>0</v>
+      </c>
+      <c r="G50" s="55" t="s">
+        <v>122</v>
+      </c>
+      <c r="H50" s="55"/>
+    </row>
+    <row r="51" spans="2:8" ht="32" x14ac:dyDescent="0.2">
       <c r="B51" s="17">
         <v>49</v>
       </c>
@@ -3121,39 +2854,41 @@
         <v>2012</v>
       </c>
       <c r="D51" s="20" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="E51" s="23" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="F51" s="18">
         <v>0</v>
       </c>
       <c r="G51" s="19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="52" spans="2:7" ht="30">
-      <c r="B52" s="54">
+        <v>122</v>
+      </c>
+      <c r="H51" s="19"/>
+    </row>
+    <row r="52" spans="2:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="B52" s="52">
         <v>50</v>
       </c>
-      <c r="C52" s="55">
+      <c r="C52" s="53">
         <v>2012</v>
       </c>
-      <c r="D52" s="62" t="s">
-        <v>106</v>
-      </c>
-      <c r="E52" s="60" t="s">
-        <v>107</v>
-      </c>
-      <c r="F52" s="55">
-        <v>0</v>
-      </c>
-      <c r="G52" s="57" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="53" spans="2:7" ht="45">
+      <c r="D52" s="60" t="s">
+        <v>96</v>
+      </c>
+      <c r="E52" s="58" t="s">
+        <v>97</v>
+      </c>
+      <c r="F52" s="53">
+        <v>0</v>
+      </c>
+      <c r="G52" s="55" t="s">
+        <v>122</v>
+      </c>
+      <c r="H52" s="55"/>
+    </row>
+    <row r="53" spans="2:8" ht="48" x14ac:dyDescent="0.2">
       <c r="B53" s="17">
         <v>51</v>
       </c>
@@ -3161,39 +2896,41 @@
         <v>2012</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="E53" s="23" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="F53" s="18">
         <v>0</v>
       </c>
       <c r="G53" s="19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="54" spans="2:7" ht="30">
-      <c r="B54" s="54">
+        <v>122</v>
+      </c>
+      <c r="H53" s="19"/>
+    </row>
+    <row r="54" spans="2:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="B54" s="52">
         <v>52</v>
       </c>
-      <c r="C54" s="55">
+      <c r="C54" s="53">
         <v>2013</v>
       </c>
-      <c r="D54" s="56" t="s">
-        <v>112</v>
-      </c>
-      <c r="E54" s="56" t="s">
-        <v>113</v>
-      </c>
-      <c r="F54" s="55">
-        <v>0</v>
-      </c>
-      <c r="G54" s="57" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="55" spans="2:7" ht="30">
+      <c r="D54" s="54" t="s">
+        <v>101</v>
+      </c>
+      <c r="E54" s="54" t="s">
+        <v>102</v>
+      </c>
+      <c r="F54" s="53">
+        <v>0</v>
+      </c>
+      <c r="G54" s="55" t="s">
+        <v>122</v>
+      </c>
+      <c r="H54" s="55"/>
+    </row>
+    <row r="55" spans="2:8" ht="32" x14ac:dyDescent="0.2">
       <c r="B55" s="17">
         <v>53</v>
       </c>
@@ -3201,39 +2938,43 @@
         <v>2013</v>
       </c>
       <c r="D55" s="20" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E55" s="23" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="F55" s="18">
         <v>2</v>
       </c>
       <c r="G55" s="19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="56" spans="2:7" ht="30">
-      <c r="B56" s="54">
+        <v>122</v>
+      </c>
+      <c r="H55" s="19"/>
+    </row>
+    <row r="56" spans="2:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="B56" s="52">
         <v>54</v>
       </c>
-      <c r="C56" s="55">
+      <c r="C56" s="53">
         <v>2013</v>
       </c>
-      <c r="D56" s="56" t="s">
-        <v>114</v>
-      </c>
-      <c r="E56" s="56" t="s">
-        <v>111</v>
-      </c>
-      <c r="F56" s="55">
+      <c r="D56" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="E56" s="54" t="s">
+        <v>100</v>
+      </c>
+      <c r="F56" s="53">
         <v>2</v>
       </c>
-      <c r="G56" s="57" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="57" spans="2:7" ht="30">
+      <c r="G56" s="55" t="s">
+        <v>123</v>
+      </c>
+      <c r="H56" s="55" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" ht="32" x14ac:dyDescent="0.2">
       <c r="B57" s="17">
         <v>55</v>
       </c>
@@ -3241,39 +2982,41 @@
         <v>2013</v>
       </c>
       <c r="D57" s="10" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="E57" s="10" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="F57" s="18">
         <v>2</v>
       </c>
       <c r="G57" s="19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="58" spans="2:7" ht="30">
-      <c r="B58" s="54">
+        <v>122</v>
+      </c>
+      <c r="H57" s="19"/>
+    </row>
+    <row r="58" spans="2:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="B58" s="52">
         <v>56</v>
       </c>
-      <c r="C58" s="55">
+      <c r="C58" s="53">
         <v>2013</v>
       </c>
-      <c r="D58" s="56" t="s">
-        <v>117</v>
-      </c>
-      <c r="E58" s="56" t="s">
-        <v>118</v>
-      </c>
-      <c r="F58" s="55">
-        <v>0</v>
-      </c>
-      <c r="G58" s="57" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="59" spans="2:7" ht="30">
+      <c r="D58" s="54" t="s">
+        <v>106</v>
+      </c>
+      <c r="E58" s="54" t="s">
+        <v>107</v>
+      </c>
+      <c r="F58" s="53">
+        <v>0</v>
+      </c>
+      <c r="G58" s="55" t="s">
+        <v>122</v>
+      </c>
+      <c r="H58" s="55"/>
+    </row>
+    <row r="59" spans="2:8" ht="32" x14ac:dyDescent="0.2">
       <c r="B59" s="17">
         <v>57</v>
       </c>
@@ -3281,39 +3024,41 @@
         <v>2013</v>
       </c>
       <c r="D59" s="10" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="E59" s="10" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="F59" s="18">
         <v>1</v>
       </c>
       <c r="G59" s="19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="60" spans="2:7">
-      <c r="B60" s="54">
+        <v>122</v>
+      </c>
+      <c r="H59" s="19"/>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B60" s="52">
         <v>58</v>
       </c>
-      <c r="C60" s="55">
+      <c r="C60" s="53">
         <v>2013</v>
       </c>
-      <c r="D60" s="56" t="s">
-        <v>121</v>
-      </c>
-      <c r="E60" s="56" t="s">
-        <v>122</v>
-      </c>
-      <c r="F60" s="55">
-        <v>0</v>
-      </c>
-      <c r="G60" s="57" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="61" spans="2:7" ht="30">
+      <c r="D60" s="54" t="s">
+        <v>110</v>
+      </c>
+      <c r="E60" s="54" t="s">
+        <v>111</v>
+      </c>
+      <c r="F60" s="53">
+        <v>0</v>
+      </c>
+      <c r="G60" s="55" t="s">
+        <v>122</v>
+      </c>
+      <c r="H60" s="55"/>
+    </row>
+    <row r="61" spans="2:8" ht="32" x14ac:dyDescent="0.2">
       <c r="B61" s="17">
         <v>59</v>
       </c>
@@ -3321,219 +3066,43 @@
         <v>2013</v>
       </c>
       <c r="D61" s="10" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="E61" s="10" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="F61" s="18">
         <v>0</v>
       </c>
       <c r="G61" s="19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="62" spans="2:7" ht="31" thickBot="1">
-      <c r="B62" s="64">
+        <v>122</v>
+      </c>
+      <c r="H61" s="19"/>
+    </row>
+    <row r="62" spans="2:8" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="62">
         <v>60</v>
       </c>
-      <c r="C62" s="65">
+      <c r="C62" s="63">
         <v>2013</v>
       </c>
-      <c r="D62" s="66" t="s">
-        <v>125</v>
-      </c>
-      <c r="E62" s="66" t="s">
-        <v>126</v>
-      </c>
-      <c r="F62" s="65">
-        <v>0</v>
-      </c>
-      <c r="G62" s="67" t="s">
-        <v>4</v>
-      </c>
+      <c r="D62" s="64" t="s">
+        <v>114</v>
+      </c>
+      <c r="E62" s="64" t="s">
+        <v>115</v>
+      </c>
+      <c r="F62" s="63">
+        <v>0</v>
+      </c>
+      <c r="G62" s="65" t="s">
+        <v>122</v>
+      </c>
+      <c r="H62" s="65"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G8"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="4.33203125" style="15" customWidth="1"/>
-    <col min="2" max="2" width="5.1640625" style="14" customWidth="1"/>
-    <col min="3" max="3" width="8.1640625" style="14" customWidth="1"/>
-    <col min="4" max="4" width="49.6640625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="30" style="7" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" style="14" customWidth="1"/>
-    <col min="7" max="7" width="19.83203125" style="14" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="15"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:7" ht="16" thickBot="1"/>
-    <row r="2" spans="2:7" s="16" customFormat="1">
-      <c r="B2" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="29" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" ht="30">
-      <c r="B3" s="17">
-        <v>1</v>
-      </c>
-      <c r="C3" s="18">
-        <v>2011</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F3" s="18">
-        <v>2</v>
-      </c>
-      <c r="G3" s="19" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" ht="45">
-      <c r="B4" s="54">
-        <v>2</v>
-      </c>
-      <c r="C4" s="55">
-        <v>2011</v>
-      </c>
-      <c r="D4" s="62" t="s">
-        <v>65</v>
-      </c>
-      <c r="E4" s="60" t="s">
-        <v>111</v>
-      </c>
-      <c r="F4" s="55">
-        <v>2</v>
-      </c>
-      <c r="G4" s="57" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" ht="30">
-      <c r="B5" s="17">
-        <v>3</v>
-      </c>
-      <c r="C5" s="18">
-        <v>2012</v>
-      </c>
-      <c r="D5" s="68" t="s">
-        <v>78</v>
-      </c>
-      <c r="E5" s="69" t="s">
-        <v>79</v>
-      </c>
-      <c r="F5" s="18">
-        <v>2</v>
-      </c>
-      <c r="G5" s="19" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" ht="30">
-      <c r="B6" s="54">
-        <v>4</v>
-      </c>
-      <c r="C6" s="55">
-        <v>2012</v>
-      </c>
-      <c r="D6" s="58" t="s">
-        <v>98</v>
-      </c>
-      <c r="E6" s="60" t="s">
-        <v>99</v>
-      </c>
-      <c r="F6" s="55">
-        <v>2</v>
-      </c>
-      <c r="G6" s="57" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" ht="45">
-      <c r="B7" s="17">
-        <v>5</v>
-      </c>
-      <c r="C7" s="18">
-        <v>2012</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="18">
-        <v>1</v>
-      </c>
-      <c r="G7" s="19" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" ht="30">
-      <c r="B8" s="54">
-        <v>6</v>
-      </c>
-      <c r="C8" s="55">
-        <v>2013</v>
-      </c>
-      <c r="D8" s="56" t="s">
-        <v>114</v>
-      </c>
-      <c r="E8" s="56" t="s">
-        <v>111</v>
-      </c>
-      <c r="F8" s="55">
-        <v>2</v>
-      </c>
-      <c r="G8" s="57" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
File translated to English
</commit_message>
<xml_diff>
--- a/db-ciber-tri.xlsx
+++ b/db-ciber-tri.xlsx
@@ -132,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="131">
   <si>
     <t>ID</t>
   </si>
@@ -535,6 +535,9 @@
   </si>
   <si>
     <t>Copenhagen School; Liberalism</t>
+  </si>
+  <si>
+    <t>Last update: 2015-08-15</t>
   </si>
 </sst>
 </file>
@@ -1027,7 +1030,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1225,6 +1228,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="88">
@@ -1591,10 +1597,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Plan1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="B1:F10"/>
+  <dimension ref="B1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1772,6 +1778,11 @@
       <c r="F10" s="45">
         <f>E10/D10</f>
         <v>9.0225563909774431E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B12" s="68" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>